<commit_message>
just finished failing tests
</commit_message>
<xml_diff>
--- a/ICJK_ClueLayoutOfficiaI.xlsx
+++ b/ICJK_ClueLayoutOfficiaI.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26812"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan\ClueGameICJK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iancairns/Documents/306SysEng/ClueGameICJK/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10954" windowHeight="8074"/>
+    <workbookView xWindow="12040" yWindow="1740" windowWidth="14340" windowHeight="12280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="29">
   <si>
     <t>K</t>
   </si>
@@ -101,14 +104,23 @@
     <t>Purple: Adjacency List Test - Within Room</t>
   </si>
   <si>
-    <t>Red: Adjacency List Test - Doorway</t>
+    <t>hightlight yellow: walkway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dark blue: targets </t>
+  </si>
+  <si>
+    <t>orange:adjecencies room entrances</t>
+  </si>
+  <si>
+    <t>Red: Adjacency List Test - room exit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,8 +128,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,13 +179,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF99FFCC"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -185,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -202,12 +237,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -217,35 +246,35 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF017AC3"/>
       <color rgb="FF99FFCC"/>
       <color rgb="FFFF5050"/>
       <color rgb="FF9999FF"/>
       <color rgb="FF9BC2E6"/>
       <color rgb="FFFFFFCC"/>
-      <color rgb="FF017AC3"/>
       <color rgb="FFFFD4AA"/>
       <color rgb="FFFF9C47"/>
       <color rgb="FFFF6699"/>
@@ -560,15 +589,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y31"/>
+  <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="91" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -593,7 +622,7 @@
       <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -611,7 +640,7 @@
       <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="P1" s="4" t="s">
@@ -623,7 +652,7 @@
       <c r="R1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="T1" s="4" t="s">
@@ -645,7 +674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -670,7 +699,7 @@
       <c r="H2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -688,7 +717,7 @@
       <c r="N2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="P2" s="4" t="s">
@@ -700,7 +729,7 @@
       <c r="R2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="10" t="s">
+      <c r="S2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="T2" s="4" t="s">
@@ -722,7 +751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -747,7 +776,7 @@
       <c r="H3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -765,7 +794,7 @@
       <c r="N3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="P3" s="4" t="s">
@@ -777,7 +806,7 @@
       <c r="R3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="S3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="T3" s="4" t="s">
@@ -799,7 +828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -824,7 +853,7 @@
       <c r="H4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -842,7 +871,7 @@
       <c r="N4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="O4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="P4" s="4" t="s">
@@ -854,7 +883,7 @@
       <c r="R4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S4" s="10" t="s">
+      <c r="S4" s="11" t="s">
         <v>1</v>
       </c>
       <c r="T4" s="4" t="s">
@@ -876,7 +905,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -901,10 +930,10 @@
       <c r="H5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="10" t="s">
+      <c r="I5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -916,10 +945,10 @@
       <c r="M5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="O5" s="10" t="s">
+      <c r="N5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="P5" s="4" t="s">
@@ -931,7 +960,7 @@
       <c r="R5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S5" s="10" t="s">
+      <c r="S5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="T5" s="4" t="s">
@@ -953,7 +982,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -978,25 +1007,25 @@
       <c r="H6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K6" s="10" t="s">
+      <c r="I6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="O6" s="10" t="s">
+      <c r="M6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="P6" s="4" t="s">
@@ -1008,10 +1037,10 @@
       <c r="R6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="S6" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="T6" s="4" t="s">
+      <c r="S6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="T6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="U6" s="4" t="s">
@@ -1030,7 +1059,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1049,65 +1078,65 @@
       <c r="F7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="8" t="s">
+      <c r="G7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" s="10" t="s">
+      <c r="I7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="7" t="s">
         <v>1</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="O7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="P7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="R7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="S7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="T7" s="10" t="s">
+      <c r="M7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="T7" s="7" t="s">
         <v>1</v>
       </c>
       <c r="U7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="V7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="W7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="X7" s="10" t="s">
+      <c r="V7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="W7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="X7" s="7" t="s">
         <v>1</v>
       </c>
       <c r="Y7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -1132,59 +1161,59 @@
       <c r="H8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="O8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="P8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="R8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="S8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="T8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="U8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="V8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="W8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="X8" s="10" t="s">
+      <c r="I8" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="S8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="V8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="W8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="X8" s="7" t="s">
         <v>1</v>
       </c>
       <c r="Y8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -1209,59 +1238,59 @@
       <c r="H9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="N9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="O9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="P9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="R9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="S9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="T9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="U9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="V9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="W9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="X9" s="10" t="s">
+      <c r="I9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="T9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="U9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="V9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="W9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="X9" s="11" t="s">
         <v>1</v>
       </c>
       <c r="Y9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -1286,16 +1315,16 @@
       <c r="H10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L10" s="10" t="s">
+      <c r="I10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="7" t="s">
         <v>1</v>
       </c>
       <c r="M10" s="3" t="s">
@@ -1307,13 +1336,13 @@
       <c r="O10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P10" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="R10" s="10" t="s">
+      <c r="P10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R10" s="7" t="s">
         <v>1</v>
       </c>
       <c r="S10" s="4" t="s">
@@ -1338,20 +1367,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="10" t="s">
+      <c r="D11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="4" t="s">
@@ -1363,13 +1392,13 @@
       <c r="H11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K11" s="10" t="s">
+      <c r="I11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="7" t="s">
         <v>1</v>
       </c>
       <c r="L11" s="3" t="s">
@@ -1387,10 +1416,10 @@
       <c r="P11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q11" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="R11" s="10" t="s">
+      <c r="Q11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R11" s="7" t="s">
         <v>1</v>
       </c>
       <c r="S11" s="4" t="s">
@@ -1415,38 +1444,38 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" s="10" t="s">
+      <c r="B12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>1</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K12" s="10" t="s">
+      <c r="I12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="7" t="s">
         <v>1</v>
       </c>
       <c r="L12" s="3" t="s">
@@ -1464,10 +1493,10 @@
       <c r="P12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="R12" s="10" t="s">
+      <c r="Q12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R12" s="7" t="s">
         <v>1</v>
       </c>
       <c r="S12" s="4" t="s">
@@ -1492,38 +1521,38 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A13" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K13" s="10" t="s">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="7" t="s">
         <v>1</v>
       </c>
       <c r="L13" s="3" t="s">
@@ -1541,10 +1570,10 @@
       <c r="P13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q13" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="R13" s="10" t="s">
+      <c r="Q13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R13" s="7" t="s">
         <v>1</v>
       </c>
       <c r="S13" s="4" t="s">
@@ -1569,38 +1598,38 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A14" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K14" s="10" t="s">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="7" t="s">
         <v>1</v>
       </c>
       <c r="L14" s="3" t="s">
@@ -1618,16 +1647,16 @@
       <c r="P14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q14" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="R14" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="S14" s="2" t="s">
+      <c r="Q14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R14" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="S14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="T14" s="5" t="s">
+      <c r="T14" s="4" t="s">
         <v>3</v>
       </c>
       <c r="U14" s="4" t="s">
@@ -1646,7 +1675,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
@@ -1659,10 +1688,10 @@
       <c r="D15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="4" t="s">
@@ -1671,13 +1700,13 @@
       <c r="H15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K15" s="10" t="s">
+      <c r="I15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="7" t="s">
         <v>1</v>
       </c>
       <c r="L15" s="3" t="s">
@@ -1695,35 +1724,35 @@
       <c r="P15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q15" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="R15" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="S15" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="T15" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="U15" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="V15" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="W15" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="X15" s="10" t="s">
+      <c r="Q15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="T15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="U15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="V15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="W15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="X15" s="7" t="s">
         <v>1</v>
       </c>
       <c r="Y15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
@@ -1751,10 +1780,10 @@
       <c r="I16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J16" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K16" s="10" t="s">
+      <c r="J16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="7" t="s">
         <v>1</v>
       </c>
       <c r="L16" s="3" t="s">
@@ -1772,25 +1801,25 @@
       <c r="P16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q16" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="R16" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="S16" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="T16" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="U16" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="V16" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="W16" s="10" t="s">
+      <c r="Q16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="S16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="U16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="V16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="W16" s="7" t="s">
         <v>1</v>
       </c>
       <c r="X16" s="4" t="s">
@@ -1800,7 +1829,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>9</v>
       </c>
@@ -1828,10 +1857,10 @@
       <c r="I17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K17" s="10" t="s">
+      <c r="J17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="7" t="s">
         <v>1</v>
       </c>
       <c r="L17" s="3" t="s">
@@ -1849,25 +1878,25 @@
       <c r="P17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q17" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="R17" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="S17" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="T17" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="U17" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="V17" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="W17" s="2" t="s">
+      <c r="Q17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="T17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="U17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="V17" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="W17" s="6" t="s">
         <v>16</v>
       </c>
       <c r="X17" s="4" t="s">
@@ -1877,7 +1906,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
@@ -1905,13 +1934,13 @@
       <c r="I18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J18" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K18" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L18" s="10" t="s">
+      <c r="J18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" s="7" t="s">
         <v>1</v>
       </c>
       <c r="M18" s="3" t="s">
@@ -1923,19 +1952,19 @@
       <c r="O18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P18" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="R18" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="S18" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="T18" s="10" t="s">
+      <c r="P18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="S18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="T18" s="7" t="s">
         <v>1</v>
       </c>
       <c r="U18" s="4" t="s">
@@ -1954,7 +1983,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>9</v>
       </c>
@@ -1967,7 +1996,7 @@
       <c r="D19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="12" t="s">
         <v>20</v>
       </c>
       <c r="F19" s="4" t="s">
@@ -1982,37 +2011,37 @@
       <c r="I19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J19" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K19" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L19" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="M19" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="N19" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="O19" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="P19" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="R19" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="S19" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="T19" s="4" t="s">
+      <c r="J19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="T19" s="5" t="s">
         <v>0</v>
       </c>
       <c r="U19" s="4" t="s">
@@ -2031,62 +2060,62 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A20" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J20" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K20" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L20" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="M20" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="N20" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="O20" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="P20" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="R20" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="S20" s="10" t="s">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="S20" s="7" t="s">
         <v>1</v>
       </c>
       <c r="T20" s="4" t="s">
@@ -2108,59 +2137,59 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="I21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="M21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="N21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="O21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="P21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="R21" s="10" t="s">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R21" s="7" t="s">
         <v>1</v>
       </c>
       <c r="S21" s="4" t="s">
@@ -2185,7 +2214,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>5</v>
       </c>
@@ -2201,43 +2230,43 @@
       <c r="E22" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J22" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K22" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="L22" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="M22" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="N22" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="O22" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="P22" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="R22" s="10" t="s">
+      <c r="F22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M22" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="R22" s="7" t="s">
         <v>1</v>
       </c>
       <c r="S22" s="4" t="s">
@@ -2262,7 +2291,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>5</v>
       </c>
@@ -2278,19 +2307,19 @@
       <c r="E23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G23" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H23" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="I23" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J23" s="10" t="s">
+      <c r="G23" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" s="7" t="s">
         <v>1</v>
       </c>
       <c r="K23" s="4" t="s">
@@ -2302,16 +2331,16 @@
       <c r="M23" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N23" s="4" t="s">
+      <c r="N23" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="O23" s="5" t="s">
+      <c r="O23" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="P23" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="10" t="s">
+      <c r="P23" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="7" t="s">
         <v>1</v>
       </c>
       <c r="R23" s="4" t="s">
@@ -2339,7 +2368,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
@@ -2358,16 +2387,16 @@
       <c r="F24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H24" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J24" s="10" t="s">
+      <c r="G24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J24" s="7" t="s">
         <v>1</v>
       </c>
       <c r="K24" s="4" t="s">
@@ -2376,7 +2405,7 @@
       <c r="L24" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M24" s="4" t="s">
+      <c r="M24" s="9" t="s">
         <v>2</v>
       </c>
       <c r="N24" s="4" t="s">
@@ -2385,7 +2414,7 @@
       <c r="O24" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="P24" s="10" t="s">
+      <c r="P24" s="7" t="s">
         <v>1</v>
       </c>
       <c r="Q24" s="2" t="s">
@@ -2416,7 +2445,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>5</v>
       </c>
@@ -2438,13 +2467,13 @@
       <c r="G25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H25" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J25" s="10" t="s">
+      <c r="H25" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J25" s="7" t="s">
         <v>1</v>
       </c>
       <c r="K25" s="4" t="s">
@@ -2453,7 +2482,7 @@
       <c r="L25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M25" s="4" t="s">
+      <c r="M25" s="5" t="s">
         <v>2</v>
       </c>
       <c r="N25" s="4" t="s">
@@ -2462,7 +2491,7 @@
       <c r="O25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="P25" s="10" t="s">
+      <c r="P25" s="7" t="s">
         <v>1</v>
       </c>
       <c r="Q25" s="4" t="s">
@@ -2493,7 +2522,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>5</v>
       </c>
@@ -2518,10 +2547,10 @@
       <c r="H26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I26" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J26" s="10" t="s">
+      <c r="I26" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J26" s="7" t="s">
         <v>1</v>
       </c>
       <c r="K26" s="4" t="s">
@@ -2539,7 +2568,7 @@
       <c r="O26" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="P26" s="10" t="s">
+      <c r="P26" s="12" t="s">
         <v>1</v>
       </c>
       <c r="Q26" s="4" t="s">
@@ -2563,14 +2592,14 @@
       <c r="W26" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="X26" s="5" t="s">
+      <c r="X26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="Y26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>0</v>
       </c>
@@ -2644,23 +2673,38 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A29" s="6" t="s">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A30" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A31" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A32" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>